<commit_message>
FLUXO DE CAIXA DO DIA 05/09/2019
</commit_message>
<xml_diff>
--- a/FLUXO DE CAIXA AGOSTO 2019/02-09-2019_FluxoDeCaixa.xlsx
+++ b/FLUXO DE CAIXA AGOSTO 2019/02-09-2019_FluxoDeCaixa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natal\OneDrive\Documentos\GitHub\ConnectFibra\FLUXO DE CAIXA AGOSTO 2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C80FBFD-B70F-4E6D-AE85-726173F5BCDD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D64C065-B8DF-4C34-9F62-5C5BCD06866B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9152A456-9720-4D0C-842A-50118CAD28D0}"/>
   </bookViews>
@@ -178,11 +178,11 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -515,10 +515,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -607,7 +607,7 @@
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>82.5</v>
       </c>
     </row>
@@ -615,7 +615,7 @@
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>140</v>
       </c>
     </row>
@@ -623,7 +623,7 @@
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>5</v>
       </c>
     </row>
@@ -631,7 +631,7 @@
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>1144</v>
       </c>
     </row>

</xml_diff>